<commit_message>
Sprint 1 # Proyecto Urban Routes
</commit_message>
<xml_diff>
--- a/Axel Arturo Contreras Van Dyck, Grupo 14 - 1.er sprint.xlsx
+++ b/Axel Arturo Contreras Van Dyck, Grupo 14 - 1.er sprint.xlsx
@@ -8,7 +8,8 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="G:\My Drive\TripleTen Projects\Sprint 1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{093BF0B0-BC8B-491E-9BAD-ECF42BC94ED6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A6B0D9B4-8AA0-4D1E-9675-319B287B0429}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <workbookProtection workbookAlgorithmName="SHA-512" workbookHashValue="h1SH4aqtYqXKzkeWNaQSgn6BHz48R+FIuIHBqMtRQMoE+x3lggRYR0v0sg4ICgKximl3Xf0MCBz+aSHyW9d2bg==" workbookSaltValue="k+zdE32r8pIBZeRGB+VLIw==" workbookSpinCount="100000" lockStructure="1"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -1094,11 +1095,11 @@
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -1388,13 +1389,13 @@
       <c r="H2" s="6"/>
     </row>
     <row r="3" spans="1:8" ht="50.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>14</v>
       </c>
-      <c r="B3" s="12" t="s">
+      <c r="B3" s="14" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="12" t="s">
+      <c r="C3" s="14" t="s">
         <v>16</v>
       </c>
       <c r="D3" s="5">
@@ -1403,13 +1404,13 @@
       <c r="E3" s="5" t="s">
         <v>10</v>
       </c>
-      <c r="F3" s="12" t="s">
+      <c r="F3" s="14" t="s">
         <v>17</v>
       </c>
-      <c r="G3" s="14" t="s">
+      <c r="G3" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H3" s="14"/>
+      <c r="H3" s="12"/>
     </row>
     <row r="4" spans="1:8" ht="49.5" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="13"/>
@@ -1500,10 +1501,10 @@
       <c r="H7" s="6"/>
     </row>
     <row r="8" spans="1:8" ht="32.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="12" t="s">
+      <c r="A8" s="14" t="s">
         <v>33</v>
       </c>
-      <c r="B8" s="12" t="s">
+      <c r="B8" s="14" t="s">
         <v>34</v>
       </c>
       <c r="C8" s="5" t="s">
@@ -1515,13 +1516,13 @@
       <c r="E8" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F8" s="12" t="s">
+      <c r="F8" s="14" t="s">
         <v>36</v>
       </c>
-      <c r="G8" s="14" t="s">
+      <c r="G8" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H8" s="14" t="s">
+      <c r="H8" s="12" t="s">
         <v>37</v>
       </c>
     </row>
@@ -1542,10 +1543,10 @@
       <c r="H9" s="13"/>
     </row>
     <row r="10" spans="1:8" ht="41.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="12" t="s">
+      <c r="A10" s="14" t="s">
         <v>39</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="14" t="s">
         <v>40</v>
       </c>
       <c r="C10" s="5" t="s">
@@ -1557,13 +1558,13 @@
       <c r="E10" s="5" t="s">
         <v>31</v>
       </c>
-      <c r="F10" s="12" t="s">
+      <c r="F10" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G10" s="14" t="s">
+      <c r="G10" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="14" t="s">
+      <c r="H10" s="12" t="s">
         <v>42</v>
       </c>
     </row>
@@ -1584,10 +1585,10 @@
       <c r="H11" s="13"/>
     </row>
     <row r="12" spans="1:8" ht="25.5" x14ac:dyDescent="0.2">
-      <c r="A12" s="12" t="s">
+      <c r="A12" s="14" t="s">
         <v>45</v>
       </c>
-      <c r="B12" s="12" t="s">
+      <c r="B12" s="14" t="s">
         <v>46</v>
       </c>
       <c r="C12" s="5" t="s">
@@ -1599,13 +1600,13 @@
       <c r="E12" s="5" t="s">
         <v>35</v>
       </c>
-      <c r="F12" s="12" t="s">
+      <c r="F12" s="14" t="s">
         <v>41</v>
       </c>
-      <c r="G12" s="14" t="s">
+      <c r="G12" s="12" t="s">
         <v>23</v>
       </c>
-      <c r="H12" s="14" t="s">
+      <c r="H12" s="12" t="s">
         <v>47</v>
       </c>
     </row>
@@ -1748,10 +1749,10 @@
       <c r="H18" s="6"/>
     </row>
     <row r="19" spans="1:9" ht="63" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="12" t="s">
+      <c r="A19" s="14" t="s">
         <v>73</v>
       </c>
-      <c r="B19" s="12" t="s">
+      <c r="B19" s="14" t="s">
         <v>74</v>
       </c>
       <c r="C19" s="5" t="s">
@@ -1763,13 +1764,13 @@
       <c r="E19" s="5" t="s">
         <v>75</v>
       </c>
-      <c r="F19" s="12" t="s">
+      <c r="F19" s="14" t="s">
         <v>76</v>
       </c>
-      <c r="G19" s="14" t="s">
+      <c r="G19" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H19" s="14"/>
+      <c r="H19" s="12"/>
     </row>
     <row r="20" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13"/>
@@ -1800,10 +1801,10 @@
       <c r="H21" s="13"/>
     </row>
     <row r="22" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="12" t="s">
+      <c r="A22" s="14" t="s">
         <v>79</v>
       </c>
-      <c r="B22" s="12" t="s">
+      <c r="B22" s="14" t="s">
         <v>80</v>
       </c>
       <c r="C22" s="5" t="s">
@@ -1815,13 +1816,13 @@
       <c r="E22" s="5" t="s">
         <v>81</v>
       </c>
-      <c r="F22" s="12" t="s">
+      <c r="F22" s="14" t="s">
         <v>82</v>
       </c>
-      <c r="G22" s="14" t="s">
+      <c r="G22" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="H22" s="14"/>
+      <c r="H22" s="12"/>
     </row>
     <row r="23" spans="1:9" ht="42" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="13"/>
@@ -1986,13 +1987,13 @@
       <c r="H29" s="6"/>
     </row>
     <row r="30" spans="1:9" ht="48.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="12" t="s">
+      <c r="A30" s="14" t="s">
         <v>111</v>
       </c>
-      <c r="B30" s="12" t="s">
+      <c r="B30" s="14" t="s">
         <v>112</v>
       </c>
-      <c r="C30" s="12" t="s">
+      <c r="C30" s="14" t="s">
         <v>113</v>
       </c>
       <c r="D30" s="5">
@@ -2004,10 +2005,10 @@
       <c r="F30" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="G30" s="14" t="s">
+      <c r="G30" s="12" t="s">
         <v>88</v>
       </c>
-      <c r="H30" s="14" t="s">
+      <c r="H30" s="12" t="s">
         <v>116</v>
       </c>
       <c r="I30" s="15"/>
@@ -4895,6 +4896,27 @@
     <row r="1000" ht="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="37">
+    <mergeCell ref="A30:A34"/>
+    <mergeCell ref="B30:B34"/>
+    <mergeCell ref="C30:C34"/>
+    <mergeCell ref="A10:A11"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="A12:A13"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="A19:A21"/>
+    <mergeCell ref="B19:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="G30:G34"/>
+    <mergeCell ref="H30:H34"/>
+    <mergeCell ref="I30:I33"/>
+    <mergeCell ref="G8:G9"/>
+    <mergeCell ref="H8:H9"/>
+    <mergeCell ref="G10:G11"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="G12:G13"/>
+    <mergeCell ref="H12:H13"/>
+    <mergeCell ref="H19:H21"/>
+    <mergeCell ref="H22:H23"/>
     <mergeCell ref="H3:H4"/>
     <mergeCell ref="A8:A9"/>
     <mergeCell ref="B8:B9"/>
@@ -4911,27 +4933,6 @@
     <mergeCell ref="F10:F11"/>
     <mergeCell ref="F12:F13"/>
     <mergeCell ref="F19:F21"/>
-    <mergeCell ref="G30:G34"/>
-    <mergeCell ref="H30:H34"/>
-    <mergeCell ref="I30:I33"/>
-    <mergeCell ref="G8:G9"/>
-    <mergeCell ref="H8:H9"/>
-    <mergeCell ref="G10:G11"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="G12:G13"/>
-    <mergeCell ref="H12:H13"/>
-    <mergeCell ref="H19:H21"/>
-    <mergeCell ref="H22:H23"/>
-    <mergeCell ref="A30:A34"/>
-    <mergeCell ref="B30:B34"/>
-    <mergeCell ref="C30:C34"/>
-    <mergeCell ref="A10:A11"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="A12:A13"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="A19:A21"/>
-    <mergeCell ref="B19:B21"/>
-    <mergeCell ref="B22:B23"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0" footer="0"/>
   <pageSetup orientation="portrait"/>
@@ -4947,7 +4948,7 @@
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D2" sqref="D2"/>
+      <selection pane="bottomLeft" activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.2"/>

</xml_diff>